<commit_message>
Changed error on the residual to the error on the mean
</commit_message>
<xml_diff>
--- a/ToyQuadScan.xlsx
+++ b/ToyQuadScan.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelgrant/Documents/gm2/EDM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C737E60A-2BF4-7240-9BF2-FE1A3969404F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437CF0F3-1827-864A-93A2-55AD266A5A98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{1274A7F7-32CE-AC49-AA55-A5E18D405CEC}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{1274A7F7-32CE-AC49-AA55-A5E18D405CEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
     <sheet name="Chart2" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -250,31 +250,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-2</c:v>
+                  <c:v>-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.9393939393939394</c:v>
+                  <c:v>-2.9090909090909092</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.8823529411764706</c:v>
+                  <c:v>-2.8235294117647061</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.8285714285714285</c:v>
+                  <c:v>-2.7428571428571429</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.7777777777777777</c:v>
+                  <c:v>-2.6666666666666665</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.7297297297297298</c:v>
+                  <c:v>-2.5945945945945947</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1.6842105263157894</c:v>
+                  <c:v>-2.5263157894736841</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1.641025641025641</c:v>
+                  <c:v>-2.4615384615384617</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-1.6</c:v>
+                  <c:v>-2.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -415,31 +415,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-1.375</c:v>
+                  <c:v>-2.375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.3333333333333333</c:v>
+                  <c:v>-2.3030303030303032</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.2941176470588236</c:v>
+                  <c:v>-2.2352941176470589</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.2571428571428571</c:v>
+                  <c:v>-2.1714285714285713</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.2222222222222223</c:v>
+                  <c:v>-2.1111111111111112</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.1891891891891893</c:v>
+                  <c:v>-2.0540540540540539</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1.1578947368421053</c:v>
+                  <c:v>-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1.1282051282051282</c:v>
+                  <c:v>-1.9487179487179487</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-1.1000000000000001</c:v>
+                  <c:v>-1.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -580,31 +580,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-0.75</c:v>
+                  <c:v>-1.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.72727272727272729</c:v>
+                  <c:v>-1.696969696969697</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.70588235294117652</c:v>
+                  <c:v>-1.6470588235294117</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.68571428571428572</c:v>
+                  <c:v>-1.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.66666666666666663</c:v>
+                  <c:v>-1.5555555555555556</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.64864864864864868</c:v>
+                  <c:v>-1.5135135135135136</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.63157894736842102</c:v>
+                  <c:v>-1.4736842105263157</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.61538461538461542</c:v>
+                  <c:v>-1.4358974358974359</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.6</c:v>
+                  <c:v>-1.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -745,31 +745,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-0.125</c:v>
+                  <c:v>-1.125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.12121212121212122</c:v>
+                  <c:v>-1.0909090909090908</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.11764705882352941</c:v>
+                  <c:v>-1.0588235294117647</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.11428571428571428</c:v>
+                  <c:v>-1.0285714285714285</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.1111111111111111</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.10810810810810811</c:v>
+                  <c:v>-0.97297297297297303</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.10526315789473684</c:v>
+                  <c:v>-0.94736842105263153</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.10256410256410256</c:v>
+                  <c:v>-0.92307692307692313</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.1</c:v>
+                  <c:v>-0.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -910,31 +910,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>-0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.48484848484848486</c:v>
+                  <c:v>-0.48484848484848486</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.47058823529411764</c:v>
+                  <c:v>-0.47058823529411764</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.45714285714285713</c:v>
+                  <c:v>-0.45714285714285713</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.44444444444444442</c:v>
+                  <c:v>-0.44444444444444442</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.43243243243243246</c:v>
+                  <c:v>-0.43243243243243246</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.42105263157894735</c:v>
+                  <c:v>-0.42105263157894735</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.41025641025641024</c:v>
+                  <c:v>-0.41025641025641024</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.4</c:v>
+                  <c:v>-0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1075,31 +1075,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.125</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0909090909090908</c:v>
+                  <c:v>0.12121212121212122</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0588235294117647</c:v>
+                  <c:v>0.11764705882352941</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0285714285714285</c:v>
+                  <c:v>0.11428571428571428</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0.1111111111111111</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.97297297297297303</c:v>
+                  <c:v>0.10810810810810811</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.94736842105263153</c:v>
+                  <c:v>0.10526315789473684</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.92307692307692313</c:v>
+                  <c:v>0.10256410256410256</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.9</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1246,31 +1246,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.75</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.696969696969697</c:v>
+                  <c:v>0.72727272727272729</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6470588235294117</c:v>
+                  <c:v>0.70588235294117652</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6</c:v>
+                  <c:v>0.68571428571428572</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5555555555555556</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5135135135135136</c:v>
+                  <c:v>0.64864864864864868</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4736842105263157</c:v>
+                  <c:v>0.63157894736842102</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4358974358974359</c:v>
+                  <c:v>0.61538461538461542</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.4</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1417,31 +1417,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2.375</c:v>
+                  <c:v>1.375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3030303030303032</c:v>
+                  <c:v>1.3333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2352941176470589</c:v>
+                  <c:v>1.2941176470588236</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1714285714285713</c:v>
+                  <c:v>1.2571428571428571</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.1111111111111112</c:v>
+                  <c:v>1.2222222222222223</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0540540540540539</c:v>
+                  <c:v>1.1891891891891893</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>1.1578947368421053</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.9487179487179487</c:v>
+                  <c:v>1.1282051282051282</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.9</c:v>
+                  <c:v>1.1000000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1588,31 +1588,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.9090909090909092</c:v>
+                  <c:v>1.9393939393939394</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8235294117647061</c:v>
+                  <c:v>1.8823529411764706</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7428571428571429</c:v>
+                  <c:v>1.8285714285714285</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6666666666666665</c:v>
+                  <c:v>1.7777777777777777</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5945945945945947</c:v>
+                  <c:v>1.7297297297297298</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.5263157894736841</c:v>
+                  <c:v>1.6842105263157894</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.4615384615384617</c:v>
+                  <c:v>1.641025641025641</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.4</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3568,7 +3568,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{34F266F7-2FDF-3847-AB2E-67D25962AC7E}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="131" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3940,8 +3940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48EF844-6735-FC4F-A8F9-88668F673782}">
   <dimension ref="B1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3986,40 +3986,40 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <f>C1+$B$2</f>
-        <v>-32</v>
+        <f>C1-$B$2</f>
+        <v>-48</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:K2" si="0">D1+$B$2</f>
-        <v>-22</v>
+        <f t="shared" ref="D2:K2" si="0">D1-$B$2</f>
+        <v>-38</v>
       </c>
       <c r="E2">
         <f t="shared" si="0"/>
-        <v>-12</v>
+        <v>-28</v>
       </c>
       <c r="F2">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>-18</v>
       </c>
       <c r="G2">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="H2">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="I2">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="J2">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="K2">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
@@ -4060,39 +4060,39 @@
       </c>
       <c r="C4">
         <f>$C$2/B4</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="D4">
         <f>$D$2/B4</f>
-        <v>-1.375</v>
+        <v>-2.375</v>
       </c>
       <c r="E4">
         <f>$E$2/B4</f>
-        <v>-0.75</v>
+        <v>-1.75</v>
       </c>
       <c r="F4">
         <f>$F$2/B4</f>
-        <v>-0.125</v>
+        <v>-1.125</v>
       </c>
       <c r="G4">
         <f>$G$2/B4</f>
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="H4">
         <f>$H$2/B4</f>
-        <v>1.125</v>
+        <v>0.125</v>
       </c>
       <c r="I4">
         <f>$I$2/B4</f>
-        <v>1.75</v>
+        <v>0.75</v>
       </c>
       <c r="J4">
         <f>$J$2/B4</f>
-        <v>2.375</v>
+        <v>1.375</v>
       </c>
       <c r="K4">
         <f>$K$2/B4</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
@@ -4101,39 +4101,39 @@
       </c>
       <c r="C5">
         <f t="shared" ref="C5:C12" si="1">$C$2/B5</f>
-        <v>-1.9393939393939394</v>
+        <v>-2.9090909090909092</v>
       </c>
       <c r="D5">
         <f t="shared" ref="D5:D12" si="2">$D$2/B5</f>
-        <v>-1.3333333333333333</v>
+        <v>-2.3030303030303032</v>
       </c>
       <c r="E5">
         <f t="shared" ref="E5:E12" si="3">$E$2/B5</f>
-        <v>-0.72727272727272729</v>
+        <v>-1.696969696969697</v>
       </c>
       <c r="F5">
         <f t="shared" ref="F5:F12" si="4">$F$2/B5</f>
-        <v>-0.12121212121212122</v>
+        <v>-1.0909090909090908</v>
       </c>
       <c r="G5">
         <f t="shared" ref="G5:G12" si="5">$G$2/B5</f>
-        <v>0.48484848484848486</v>
+        <v>-0.48484848484848486</v>
       </c>
       <c r="H5">
         <f t="shared" ref="H5:H12" si="6">$H$2/B5</f>
-        <v>1.0909090909090908</v>
+        <v>0.12121212121212122</v>
       </c>
       <c r="I5">
         <f t="shared" ref="I5:I12" si="7">$I$2/B5</f>
-        <v>1.696969696969697</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="J5">
         <f t="shared" ref="J5:J12" si="8">$J$2/B5</f>
-        <v>2.3030303030303032</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="K5">
         <f t="shared" ref="K5:K12" si="9">$K$2/B5</f>
-        <v>2.9090909090909092</v>
+        <v>1.9393939393939394</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
@@ -4142,39 +4142,39 @@
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>-1.8823529411764706</v>
+        <v>-2.8235294117647061</v>
       </c>
       <c r="D6">
         <f t="shared" si="2"/>
-        <v>-1.2941176470588236</v>
+        <v>-2.2352941176470589</v>
       </c>
       <c r="E6">
         <f t="shared" si="3"/>
-        <v>-0.70588235294117652</v>
+        <v>-1.6470588235294117</v>
       </c>
       <c r="F6">
         <f t="shared" si="4"/>
-        <v>-0.11764705882352941</v>
+        <v>-1.0588235294117647</v>
       </c>
       <c r="G6">
         <f t="shared" si="5"/>
-        <v>0.47058823529411764</v>
+        <v>-0.47058823529411764</v>
       </c>
       <c r="H6">
         <f t="shared" si="6"/>
-        <v>1.0588235294117647</v>
+        <v>0.11764705882352941</v>
       </c>
       <c r="I6">
         <f t="shared" si="7"/>
-        <v>1.6470588235294117</v>
+        <v>0.70588235294117652</v>
       </c>
       <c r="J6">
         <f t="shared" si="8"/>
-        <v>2.2352941176470589</v>
+        <v>1.2941176470588236</v>
       </c>
       <c r="K6">
         <f t="shared" si="9"/>
-        <v>2.8235294117647061</v>
+        <v>1.8823529411764706</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
@@ -4183,39 +4183,39 @@
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>-1.8285714285714285</v>
+        <v>-2.7428571428571429</v>
       </c>
       <c r="D7">
         <f t="shared" si="2"/>
-        <v>-1.2571428571428571</v>
+        <v>-2.1714285714285713</v>
       </c>
       <c r="E7">
         <f t="shared" si="3"/>
-        <v>-0.68571428571428572</v>
+        <v>-1.6</v>
       </c>
       <c r="F7">
         <f t="shared" si="4"/>
-        <v>-0.11428571428571428</v>
+        <v>-1.0285714285714285</v>
       </c>
       <c r="G7">
         <f t="shared" si="5"/>
-        <v>0.45714285714285713</v>
+        <v>-0.45714285714285713</v>
       </c>
       <c r="H7">
         <f t="shared" si="6"/>
-        <v>1.0285714285714285</v>
+        <v>0.11428571428571428</v>
       </c>
       <c r="I7">
         <f t="shared" si="7"/>
-        <v>1.6</v>
+        <v>0.68571428571428572</v>
       </c>
       <c r="J7">
         <f t="shared" si="8"/>
-        <v>2.1714285714285713</v>
+        <v>1.2571428571428571</v>
       </c>
       <c r="K7">
         <f t="shared" si="9"/>
-        <v>2.7428571428571429</v>
+        <v>1.8285714285714285</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
@@ -4224,39 +4224,39 @@
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>-1.7777777777777777</v>
+        <v>-2.6666666666666665</v>
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
-        <v>-1.2222222222222223</v>
+        <v>-2.1111111111111112</v>
       </c>
       <c r="E8">
         <f t="shared" si="3"/>
-        <v>-0.66666666666666663</v>
+        <v>-1.5555555555555556</v>
       </c>
       <c r="F8">
         <f t="shared" si="4"/>
-        <v>-0.1111111111111111</v>
+        <v>-1</v>
       </c>
       <c r="G8">
         <f t="shared" si="5"/>
-        <v>0.44444444444444442</v>
+        <v>-0.44444444444444442</v>
       </c>
       <c r="H8">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="I8">
         <f t="shared" si="7"/>
-        <v>1.5555555555555556</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="J8">
         <f t="shared" si="8"/>
-        <v>2.1111111111111112</v>
+        <v>1.2222222222222223</v>
       </c>
       <c r="K8">
         <f t="shared" si="9"/>
-        <v>2.6666666666666665</v>
+        <v>1.7777777777777777</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
@@ -4265,39 +4265,39 @@
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>-1.7297297297297298</v>
+        <v>-2.5945945945945947</v>
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
-        <v>-1.1891891891891893</v>
+        <v>-2.0540540540540539</v>
       </c>
       <c r="E9">
         <f t="shared" si="3"/>
-        <v>-0.64864864864864868</v>
+        <v>-1.5135135135135136</v>
       </c>
       <c r="F9">
         <f t="shared" si="4"/>
-        <v>-0.10810810810810811</v>
+        <v>-0.97297297297297303</v>
       </c>
       <c r="G9">
         <f t="shared" si="5"/>
-        <v>0.43243243243243246</v>
+        <v>-0.43243243243243246</v>
       </c>
       <c r="H9">
         <f t="shared" si="6"/>
-        <v>0.97297297297297303</v>
+        <v>0.10810810810810811</v>
       </c>
       <c r="I9">
         <f t="shared" si="7"/>
-        <v>1.5135135135135136</v>
+        <v>0.64864864864864868</v>
       </c>
       <c r="J9">
         <f t="shared" si="8"/>
-        <v>2.0540540540540539</v>
+        <v>1.1891891891891893</v>
       </c>
       <c r="K9">
         <f t="shared" si="9"/>
-        <v>2.5945945945945947</v>
+        <v>1.7297297297297298</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
@@ -4306,39 +4306,39 @@
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>-1.6842105263157894</v>
+        <v>-2.5263157894736841</v>
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>-1.1578947368421053</v>
+        <v>-2</v>
       </c>
       <c r="E10">
         <f t="shared" si="3"/>
-        <v>-0.63157894736842102</v>
+        <v>-1.4736842105263157</v>
       </c>
       <c r="F10">
         <f t="shared" si="4"/>
-        <v>-0.10526315789473684</v>
+        <v>-0.94736842105263153</v>
       </c>
       <c r="G10">
         <f t="shared" si="5"/>
-        <v>0.42105263157894735</v>
+        <v>-0.42105263157894735</v>
       </c>
       <c r="H10">
         <f t="shared" si="6"/>
-        <v>0.94736842105263153</v>
+        <v>0.10526315789473684</v>
       </c>
       <c r="I10">
         <f t="shared" si="7"/>
-        <v>1.4736842105263157</v>
+        <v>0.63157894736842102</v>
       </c>
       <c r="J10">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1.1578947368421053</v>
       </c>
       <c r="K10">
         <f t="shared" si="9"/>
-        <v>2.5263157894736841</v>
+        <v>1.6842105263157894</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
@@ -4347,39 +4347,39 @@
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>-1.641025641025641</v>
+        <v>-2.4615384615384617</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>-1.1282051282051282</v>
+        <v>-1.9487179487179487</v>
       </c>
       <c r="E11">
         <f t="shared" si="3"/>
-        <v>-0.61538461538461542</v>
+        <v>-1.4358974358974359</v>
       </c>
       <c r="F11">
         <f t="shared" si="4"/>
-        <v>-0.10256410256410256</v>
+        <v>-0.92307692307692313</v>
       </c>
       <c r="G11">
         <f t="shared" si="5"/>
-        <v>0.41025641025641024</v>
+        <v>-0.41025641025641024</v>
       </c>
       <c r="H11">
         <f t="shared" si="6"/>
-        <v>0.92307692307692313</v>
+        <v>0.10256410256410256</v>
       </c>
       <c r="I11">
         <f t="shared" si="7"/>
-        <v>1.4358974358974359</v>
+        <v>0.61538461538461542</v>
       </c>
       <c r="J11">
         <f t="shared" si="8"/>
-        <v>1.9487179487179487</v>
+        <v>1.1282051282051282</v>
       </c>
       <c r="K11">
         <f t="shared" si="9"/>
-        <v>2.4615384615384617</v>
+        <v>1.641025641025641</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
@@ -4388,39 +4388,39 @@
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>-1.6</v>
+        <v>-2.4</v>
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>-1.1000000000000001</v>
+        <v>-1.9</v>
       </c>
       <c r="E12">
         <f t="shared" si="3"/>
-        <v>-0.6</v>
+        <v>-1.4</v>
       </c>
       <c r="F12">
         <f t="shared" si="4"/>
-        <v>-0.1</v>
+        <v>-0.9</v>
       </c>
       <c r="G12">
         <f t="shared" si="5"/>
-        <v>0.4</v>
+        <v>-0.4</v>
       </c>
       <c r="H12">
         <f t="shared" si="6"/>
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
       <c r="I12">
         <f t="shared" si="7"/>
-        <v>1.4</v>
+        <v>0.6</v>
       </c>
       <c r="J12">
         <f t="shared" si="8"/>
-        <v>1.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K12">
         <f t="shared" si="9"/>
-        <v>2.4</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Finished radial field scan 1, data taking
</commit_message>
<xml_diff>
--- a/ToyQuadScan.xlsx
+++ b/ToyQuadScan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelgrant/Documents/gm2/EDM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A92D52-2780-4C49-B291-6214CF99F0FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AA715C-8302-FF46-9E3F-1AE3800A1721}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="3" xr2:uid="{1274A7F7-32CE-AC49-AA55-A5E18D405CEC}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{1274A7F7-32CE-AC49-AA55-A5E18D405CEC}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="4" r:id="rId1"/>
@@ -8494,7 +8494,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{E898D1E5-7BE5-304D-82E4-34C404304AD1}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="136" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8978,8 +8978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C671A7EB-6A5B-7D4D-8E6B-5C021871A75D}">
   <dimension ref="B1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="B1:K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10340,15 +10340,15 @@
         <v>14.693877551020407</v>
       </c>
       <c r="G33">
-        <f>$B$9/$B$5</f>
+        <f t="shared" ref="G33:G56" si="6">$B$9/$B$5</f>
         <v>2.7142857142857144</v>
       </c>
       <c r="H33">
-        <f>$B$9*COS(E33-$B$10)/(1-$B$5)</f>
+        <f t="shared" ref="H33:H56" si="7">$B$9*COS(E33-$B$10)/(1-$B$5)</f>
         <v>-0.74145186065855972</v>
       </c>
       <c r="I33">
-        <f>$B$9*COS(2*E33-$B$11)/(4-$B$5)</f>
+        <f t="shared" ref="I33:I56" si="8">$B$9*COS(2*E33-$B$11)/(4-$B$5)</f>
         <v>-1.8647266976149641</v>
       </c>
       <c r="J33">
@@ -10367,27 +10367,27 @@
         <v>2</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E56" si="6">D34*2*PI()/(24.5)</f>
+        <f t="shared" ref="E34:E56" si="9">D34*2*PI()/(24.5)</f>
         <v>0.51291308630037435</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F56" si="7">E34*(180/PI())</f>
+        <f t="shared" ref="F34:F56" si="10">E34*(180/PI())</f>
         <v>29.387755102040813</v>
       </c>
       <c r="G34">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="6"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H34">
-        <f>$B$9*COS(E34-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="7"/>
         <v>-1.4344051520115109</v>
       </c>
       <c r="I34">
-        <f>$B$9*COS(2*E34-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>-3.2495424994203157</v>
       </c>
       <c r="J34">
-        <f t="shared" ref="J34:J56" si="8">SUM(G34:I34)</f>
+        <f t="shared" ref="J34:J56" si="11">SUM(G34:I34)</f>
         <v>-1.9696619371461122</v>
       </c>
     </row>
@@ -10403,27 +10403,27 @@
         <v>3</v>
       </c>
       <c r="E35">
+        <f t="shared" si="9"/>
+        <v>0.76936962945056153</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" si="10"/>
+        <v>44.08163265306122</v>
+      </c>
+      <c r="G35">
         <f t="shared" si="6"/>
-        <v>0.76936962945056153</v>
-      </c>
-      <c r="F35" s="1">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H35">
         <f t="shared" si="7"/>
-        <v>44.08163265306122</v>
-      </c>
-      <c r="G35">
-        <f>$B$9/$B$5</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="H35">
-        <f>$B$9*COS(E35-$B$10)/(1-$B$5)</f>
         <v>-2.0335336094563448</v>
       </c>
       <c r="I35">
-        <f>$B$9*COS(2*E35-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>-3.7980476215626142</v>
       </c>
       <c r="J35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>-3.1172955167332446</v>
       </c>
     </row>
@@ -10439,27 +10439,27 @@
         <v>4</v>
       </c>
       <c r="E36">
+        <f t="shared" si="9"/>
+        <v>1.0258261726007487</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="10"/>
+        <v>58.775510204081627</v>
+      </c>
+      <c r="G36">
         <f t="shared" si="6"/>
-        <v>1.0258261726007487</v>
-      </c>
-      <c r="F36" s="1">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H36">
         <f t="shared" si="7"/>
-        <v>58.775510204081627</v>
-      </c>
-      <c r="G36">
-        <f>$B$9/$B$5</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="H36">
-        <f>$B$9*COS(E36-$B$10)/(1-$B$5)</f>
         <v>-2.4996480764771656</v>
       </c>
       <c r="I36">
-        <f>$B$9*COS(2*E36-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>-3.3690773642174001</v>
       </c>
       <c r="J36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>-3.1544397264088513</v>
       </c>
     </row>
@@ -10475,27 +10475,27 @@
         <v>5</v>
       </c>
       <c r="E37">
+        <f t="shared" si="9"/>
+        <v>1.282282715750936</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="10"/>
+        <v>73.469387755102048</v>
+      </c>
+      <c r="G37">
         <f t="shared" si="6"/>
-        <v>1.282282715750936</v>
-      </c>
-      <c r="F37" s="1">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H37">
         <f t="shared" si="7"/>
-        <v>73.469387755102048</v>
-      </c>
-      <c r="G37">
-        <f>$B$9/$B$5</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="H37">
-        <f>$B$9*COS(E37-$B$10)/(1-$B$5)</f>
         <v>-2.8022598781071619</v>
       </c>
       <c r="I37">
-        <f>$B$9*COS(2*E37-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>-2.0730326246000845</v>
       </c>
       <c r="J37">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>-2.161006788421532</v>
       </c>
     </row>
@@ -10504,27 +10504,27 @@
         <v>6</v>
       </c>
       <c r="E38">
+        <f t="shared" si="9"/>
+        <v>1.5387392589011231</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="10"/>
+        <v>88.16326530612244</v>
+      </c>
+      <c r="G38">
         <f t="shared" si="6"/>
-        <v>1.5387392589011231</v>
-      </c>
-      <c r="F38" s="1">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H38">
         <f t="shared" si="7"/>
-        <v>88.16326530612244</v>
-      </c>
-      <c r="G38">
-        <f>$B$9/$B$5</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="H38">
-        <f>$B$9*COS(E38-$B$10)/(1-$B$5)</f>
         <v>-2.9215750935097029</v>
       </c>
       <c r="I38">
-        <f>$B$9*COS(2*E38-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>-0.24346683592671009</v>
       </c>
       <c r="J38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>-0.45075621515069858</v>
       </c>
     </row>
@@ -10533,27 +10533,27 @@
         <v>7</v>
       </c>
       <c r="E39">
+        <f t="shared" si="9"/>
+        <v>1.7951958020513104</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="10"/>
+        <v>102.85714285714286</v>
+      </c>
+      <c r="G39">
         <f t="shared" si="6"/>
-        <v>1.7951958020513104</v>
-      </c>
-      <c r="F39" s="1">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H39">
         <f t="shared" si="7"/>
-        <v>102.85714285714286</v>
-      </c>
-      <c r="G39">
-        <f>$B$9/$B$5</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="H39">
-        <f>$B$9*COS(E39-$B$10)/(1-$B$5)</f>
         <v>-2.8497892817622534</v>
       </c>
       <c r="I39">
-        <f>$B$9*COS(2*E39-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>1.6487582086467207</v>
       </c>
       <c r="J39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1.5132546411701817</v>
       </c>
     </row>
@@ -10562,27 +10562,27 @@
         <v>8</v>
       </c>
       <c r="E40">
+        <f t="shared" si="9"/>
+        <v>2.0516523452014974</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="10"/>
+        <v>117.55102040816325</v>
+      </c>
+      <c r="G40">
         <f t="shared" si="6"/>
-        <v>2.0516523452014974</v>
-      </c>
-      <c r="F40" s="1">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H40">
         <f t="shared" si="7"/>
-        <v>117.55102040816325</v>
-      </c>
-      <c r="G40">
-        <f>$B$9/$B$5</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="H40">
-        <f>$B$9*COS(E40-$B$10)/(1-$B$5)</f>
         <v>-2.591597972474923</v>
       </c>
       <c r="I40">
-        <f>$B$9*COS(2*E40-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>3.1166545674684314</v>
       </c>
       <c r="J40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>3.2393423092792228</v>
       </c>
     </row>
@@ -10591,27 +10591,27 @@
         <v>9</v>
       </c>
       <c r="E41">
+        <f t="shared" si="9"/>
+        <v>2.3081088883516849</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="10"/>
+        <v>132.24489795918367</v>
+      </c>
+      <c r="G41">
         <f t="shared" si="6"/>
-        <v>2.3081088883516849</v>
-      </c>
-      <c r="F41" s="1">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H41">
         <f t="shared" si="7"/>
-        <v>132.24489795918367</v>
-      </c>
-      <c r="G41">
-        <f>$B$9/$B$5</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="H41">
-        <f>$B$9*COS(E41-$B$10)/(1-$B$5)</f>
         <v>-2.1638895299124603</v>
       </c>
       <c r="I41">
-        <f>$B$9*COS(2*E41-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>3.7824406292069535</v>
       </c>
       <c r="J41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>4.332836813580208</v>
       </c>
     </row>
@@ -10620,27 +10620,27 @@
         <v>10</v>
       </c>
       <c r="E42">
+        <f t="shared" si="9"/>
+        <v>2.564565431501872</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="10"/>
+        <v>146.9387755102041</v>
+      </c>
+      <c r="G42">
         <f t="shared" si="6"/>
-        <v>2.564565431501872</v>
-      </c>
-      <c r="F42" s="1">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H42">
         <f t="shared" si="7"/>
-        <v>146.9387755102041</v>
-      </c>
-      <c r="G42">
-        <f>$B$9/$B$5</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="H42">
-        <f>$B$9*COS(E42-$B$10)/(1-$B$5)</f>
         <v>-1.5946404804616034</v>
       </c>
       <c r="I42">
-        <f>$B$9*COS(2*E42-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>3.4747679674600875</v>
       </c>
       <c r="J42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>4.5944132012841985</v>
       </c>
     </row>
@@ -10649,27 +10649,27 @@
         <v>11</v>
       </c>
       <c r="E43">
+        <f t="shared" si="9"/>
+        <v>2.8210219746520586</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="10"/>
+        <v>161.63265306122446</v>
+      </c>
+      <c r="G43">
         <f t="shared" si="6"/>
-        <v>2.8210219746520586</v>
-      </c>
-      <c r="F43" s="1">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H43">
         <f t="shared" si="7"/>
-        <v>161.63265306122446</v>
-      </c>
-      <c r="G43">
-        <f>$B$9/$B$5</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="H43">
-        <f>$B$9*COS(E43-$B$10)/(1-$B$5)</f>
         <v>-0.92108556037673894</v>
       </c>
       <c r="I43">
-        <f>$B$9*COS(2*E43-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>2.2728200158666239</v>
       </c>
       <c r="J43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>4.0660201697755998</v>
       </c>
     </row>
@@ -10678,27 +10678,27 @@
         <v>12</v>
       </c>
       <c r="E44">
+        <f t="shared" si="9"/>
+        <v>3.0774785178022461</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="10"/>
+        <v>176.32653061224488</v>
+      </c>
+      <c r="G44">
         <f t="shared" si="6"/>
-        <v>3.0774785178022461</v>
-      </c>
-      <c r="F44" s="1">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H44">
         <f t="shared" si="7"/>
-        <v>176.32653061224488</v>
-      </c>
-      <c r="G44">
-        <f>$B$9/$B$5</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="H44">
-        <f>$B$9*COS(E44-$B$10)/(1-$B$5)</f>
         <v>-0.18728218148208467</v>
       </c>
       <c r="I44">
-        <f>$B$9*COS(2*E44-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>0.48593321440112491</v>
       </c>
       <c r="J44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>3.0129367472047548</v>
       </c>
     </row>
@@ -10707,27 +10707,27 @@
         <v>13</v>
       </c>
       <c r="E45">
+        <f t="shared" si="9"/>
+        <v>3.3339350609524336</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="10"/>
+        <v>191.0204081632653</v>
+      </c>
+      <c r="G45">
         <f t="shared" si="6"/>
-        <v>3.3339350609524336</v>
-      </c>
-      <c r="F45" s="1">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H45">
         <f t="shared" si="7"/>
-        <v>191.0204081632653</v>
-      </c>
-      <c r="G45">
-        <f>$B$9/$B$5</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="H45">
-        <f>$B$9*COS(E45-$B$10)/(1-$B$5)</f>
         <v>0.55877137620401141</v>
       </c>
       <c r="I45">
-        <f>$B$9*COS(2*E45-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>-1.426014618541622</v>
       </c>
       <c r="J45">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1.8470424719481036</v>
       </c>
     </row>
@@ -10736,27 +10736,27 @@
         <v>14</v>
       </c>
       <c r="E46">
+        <f t="shared" si="9"/>
+        <v>3.5903916041026207</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="10"/>
+        <v>205.71428571428572</v>
+      </c>
+      <c r="G46">
         <f t="shared" si="6"/>
-        <v>3.5903916041026207</v>
-      </c>
-      <c r="F46" s="1">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H46">
         <f t="shared" si="7"/>
-        <v>205.71428571428572</v>
-      </c>
-      <c r="G46">
-        <f>$B$9/$B$5</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="H46">
-        <f>$B$9*COS(E46-$B$10)/(1-$B$5)</f>
         <v>1.268275545112862</v>
       </c>
       <c r="I46">
-        <f>$B$9*COS(2*E46-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>-2.9709596333785129</v>
       </c>
       <c r="J46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1.0116016260200635</v>
       </c>
     </row>
@@ -10765,27 +10765,27 @@
         <v>15</v>
       </c>
       <c r="E47">
+        <f t="shared" si="9"/>
+        <v>3.8468481472528078</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="10"/>
+        <v>220.40816326530611</v>
+      </c>
+      <c r="G47">
         <f t="shared" si="6"/>
-        <v>3.8468481472528078</v>
-      </c>
-      <c r="F47" s="1">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H47">
         <f t="shared" si="7"/>
-        <v>220.40816326530611</v>
-      </c>
-      <c r="G47">
-        <f>$B$9/$B$5</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="H47">
-        <f>$B$9*COS(E47-$B$10)/(1-$B$5)</f>
         <v>1.894821463207381</v>
       </c>
       <c r="I47">
-        <f>$B$9*COS(2*E47-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>-3.7512907769749106</v>
       </c>
       <c r="J47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.85781640051818497</v>
       </c>
     </row>
@@ -10794,27 +10794,27 @@
         <v>16</v>
       </c>
       <c r="E48">
+        <f t="shared" si="9"/>
+        <v>4.1033046904029948</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="10"/>
+        <v>235.10204081632651</v>
+      </c>
+      <c r="G48">
         <f t="shared" si="6"/>
-        <v>4.1033046904029948</v>
-      </c>
-      <c r="F48" s="1">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H48">
         <f t="shared" si="7"/>
-        <v>235.10204081632651</v>
-      </c>
-      <c r="G48">
-        <f>$B$9/$B$5</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="H48">
-        <f>$B$9*COS(E48-$B$10)/(1-$B$5)</f>
         <v>2.397426590360332</v>
       </c>
       <c r="I48">
-        <f>$B$9*COS(2*E48-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>-3.5661800037890905</v>
       </c>
       <c r="J48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1.5455323008569555</v>
       </c>
     </row>
@@ -10823,27 +10823,27 @@
         <v>17</v>
       </c>
       <c r="E49">
+        <f t="shared" si="9"/>
+        <v>4.3597612335531828</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="10"/>
+        <v>249.79591836734696</v>
+      </c>
+      <c r="G49">
         <f t="shared" si="6"/>
-        <v>4.3597612335531828</v>
-      </c>
-      <c r="F49" s="1">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H49">
         <f t="shared" si="7"/>
-        <v>249.79591836734696</v>
-      </c>
-      <c r="G49">
-        <f>$B$9/$B$5</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="H49">
-        <f>$B$9*COS(E49-$B$10)/(1-$B$5)</f>
         <v>2.7432153875300691</v>
       </c>
       <c r="I49">
-        <f>$B$9*COS(2*E49-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>-2.4632679021695938</v>
       </c>
       <c r="J49">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.9942331996461893</v>
       </c>
     </row>
@@ -10852,27 +10852,27 @@
         <v>18</v>
       </c>
       <c r="E50">
+        <f t="shared" si="9"/>
+        <v>4.6162177767033699</v>
+      </c>
+      <c r="F50" s="1">
+        <f t="shared" si="10"/>
+        <v>264.48979591836735</v>
+      </c>
+      <c r="G50">
         <f t="shared" si="6"/>
-        <v>4.6162177767033699</v>
-      </c>
-      <c r="F50" s="1">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H50">
         <f t="shared" si="7"/>
-        <v>264.48979591836735</v>
-      </c>
-      <c r="G50">
-        <f>$B$9/$B$5</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="H50">
-        <f>$B$9*COS(E50-$B$10)/(1-$B$5)</f>
         <v>2.9095697147745794</v>
       </c>
       <c r="I50">
-        <f>$B$9*COS(2*E50-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>-0.72640278906521305</v>
       </c>
       <c r="J50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>4.8974526399950804</v>
       </c>
     </row>
@@ -10881,27 +10881,27 @@
         <v>19</v>
       </c>
       <c r="E51">
+        <f t="shared" si="9"/>
+        <v>4.872674319853556</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="10"/>
+        <v>279.18367346938771</v>
+      </c>
+      <c r="G51">
         <f t="shared" si="6"/>
-        <v>4.872674319853556</v>
-      </c>
-      <c r="F51" s="1">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H51">
         <f t="shared" si="7"/>
-        <v>279.18367346938771</v>
-      </c>
-      <c r="G51">
-        <f>$B$9/$B$5</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="H51">
-        <f>$B$9*COS(E51-$B$10)/(1-$B$5)</f>
         <v>2.8856082899807012</v>
       </c>
       <c r="I51">
-        <f>$B$9*COS(2*E51-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>1.1974112284897527</v>
       </c>
       <c r="J51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>6.7973052327561678</v>
       </c>
     </row>
@@ -10910,27 +10910,27 @@
         <v>20</v>
       </c>
       <c r="E52">
+        <f t="shared" si="9"/>
+        <v>5.129130863003744</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="10"/>
+        <v>293.87755102040819</v>
+      </c>
+      <c r="G52">
         <f t="shared" si="6"/>
-        <v>5.129130863003744</v>
-      </c>
-      <c r="F52" s="1">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H52">
         <f t="shared" si="7"/>
-        <v>293.87755102040819</v>
-      </c>
-      <c r="G52">
-        <f>$B$9/$B$5</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="H52">
-        <f>$B$9*COS(E52-$B$10)/(1-$B$5)</f>
         <v>2.6728984365077597</v>
       </c>
       <c r="I52">
-        <f>$B$9*COS(2*E52-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>2.8130563888861988</v>
       </c>
       <c r="J52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>8.2002405396796725</v>
       </c>
     </row>
@@ -10939,27 +10939,27 @@
         <v>21</v>
       </c>
       <c r="E53">
+        <f t="shared" si="9"/>
+        <v>5.3855874061539311</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="10"/>
+        <v>308.57142857142856</v>
+      </c>
+      <c r="G53">
         <f t="shared" si="6"/>
-        <v>5.3855874061539311</v>
-      </c>
-      <c r="F53" s="1">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H53">
         <f t="shared" si="7"/>
-        <v>308.57142857142856</v>
-      </c>
-      <c r="G53">
-        <f>$B$9/$B$5</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="H53">
-        <f>$B$9*COS(E53-$B$10)/(1-$B$5)</f>
         <v>2.2853535641373179</v>
       </c>
       <c r="I53">
-        <f>$B$9*COS(2*E53-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>3.7047260662909296</v>
       </c>
       <c r="J53">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>8.7043653447139615</v>
       </c>
     </row>
@@ -10968,27 +10968,27 @@
         <v>22</v>
       </c>
       <c r="E54">
+        <f t="shared" si="9"/>
+        <v>5.6420439493041172</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="10"/>
+        <v>323.26530612244892</v>
+      </c>
+      <c r="G54">
         <f t="shared" si="6"/>
-        <v>5.6420439493041172</v>
-      </c>
-      <c r="F54" s="1">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H54">
         <f t="shared" si="7"/>
-        <v>323.26530612244892</v>
-      </c>
-      <c r="G54">
-        <f>$B$9/$B$5</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="H54">
-        <f>$B$9*COS(E54-$B$10)/(1-$B$5)</f>
         <v>1.7483230891281722</v>
       </c>
       <c r="I54">
-        <f>$B$9*COS(2*E54-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>3.6429378415393132</v>
       </c>
       <c r="J54">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>8.1055466449532005</v>
       </c>
     </row>
@@ -10997,27 +10997,27 @@
         <v>23</v>
       </c>
       <c r="E55">
+        <f t="shared" si="9"/>
+        <v>5.8985004924543052</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="10"/>
+        <v>337.9591836734694</v>
+      </c>
+      <c r="G55">
         <f t="shared" si="6"/>
-        <v>5.8985004924543052</v>
-      </c>
-      <c r="F55" s="1">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H55">
         <f t="shared" si="7"/>
-        <v>337.9591836734694</v>
-      </c>
-      <c r="G55">
-        <f>$B$9/$B$5</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="H55">
-        <f>$B$9*COS(E55-$B$10)/(1-$B$5)</f>
         <v>1.0969343219550949</v>
       </c>
       <c r="I55">
-        <f>$B$9*COS(2*E55-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>2.6435936922932508</v>
       </c>
       <c r="J55">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>6.4548137285340594</v>
       </c>
     </row>
@@ -11026,27 +11026,27 @@
         <v>24</v>
       </c>
       <c r="E56">
+        <f t="shared" si="9"/>
+        <v>6.1549570356044923</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="10"/>
+        <v>352.65306122448976</v>
+      </c>
+      <c r="G56">
         <f t="shared" si="6"/>
-        <v>6.1549570356044923</v>
-      </c>
-      <c r="F56" s="1">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H56">
         <f t="shared" si="7"/>
-        <v>352.65306122448976</v>
-      </c>
-      <c r="G56">
-        <f>$B$9/$B$5</f>
-        <v>2.7142857142857144</v>
-      </c>
-      <c r="H56">
-        <f>$B$9*COS(E56-$B$10)/(1-$B$5)</f>
         <v>0.37379478030855762</v>
       </c>
       <c r="I56">
-        <f>$B$9*COS(2*E56-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="8"/>
         <v>0.96388741885613238</v>
       </c>
       <c r="J56">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>4.0519679134504045</v>
       </c>
     </row>
@@ -11098,15 +11098,15 @@
         <v>14.693877551020407</v>
       </c>
       <c r="G59">
-        <f>$B$9/$B$5</f>
+        <f t="shared" ref="G59:G82" si="12">$B$9/$B$5</f>
         <v>2.7142857142857144</v>
       </c>
       <c r="H59">
-        <f>$B$9*COS(E59-$B$10)/(1-$B$5)</f>
+        <f t="shared" ref="H59:H82" si="13">$B$9*COS(E59-$B$10)/(1-$B$5)</f>
         <v>-0.74145186065855972</v>
       </c>
       <c r="I59">
-        <f>$B$9*COS(2*E59-$B$11)/(4-$B$5)</f>
+        <f t="shared" ref="I59:I82" si="14">$B$9*COS(2*E59-$B$11)/(4-$B$5)</f>
         <v>-1.8647266976149641</v>
       </c>
       <c r="J59">
@@ -11125,27 +11125,27 @@
         <v>2</v>
       </c>
       <c r="E60">
-        <f t="shared" ref="E60:E82" si="9">D60*2*PI()/(24.5)</f>
+        <f t="shared" ref="E60:E82" si="15">D60*2*PI()/(24.5)</f>
         <v>0.51291308630037435</v>
       </c>
       <c r="F60" s="1">
-        <f t="shared" ref="F60:F82" si="10">E60*(180/PI())</f>
+        <f t="shared" ref="F60:F82" si="16">E60*(180/PI())</f>
         <v>29.387755102040813</v>
       </c>
       <c r="G60">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H60">
-        <f>$B$9*COS(E60-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>-1.4344051520115109</v>
       </c>
       <c r="I60">
-        <f>$B$9*COS(2*E60-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>-3.2495424994203157</v>
       </c>
       <c r="J60">
-        <f t="shared" ref="J60:J82" si="11">SUM(G60:I60)</f>
+        <f t="shared" ref="J60:J82" si="17">SUM(G60:I60)</f>
         <v>-1.9696619371461122</v>
       </c>
     </row>
@@ -11161,27 +11161,27 @@
         <v>3</v>
       </c>
       <c r="E61">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>0.76936962945056153</v>
       </c>
       <c r="F61" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>44.08163265306122</v>
       </c>
       <c r="G61">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H61">
-        <f>$B$9*COS(E61-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>-2.0335336094563448</v>
       </c>
       <c r="I61">
-        <f>$B$9*COS(2*E61-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>-3.7980476215626142</v>
       </c>
       <c r="J61">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>-3.1172955167332446</v>
       </c>
     </row>
@@ -11197,27 +11197,27 @@
         <v>4</v>
       </c>
       <c r="E62">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1.0258261726007487</v>
       </c>
       <c r="F62" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>58.775510204081627</v>
       </c>
       <c r="G62">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H62">
-        <f>$B$9*COS(E62-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>-2.4996480764771656</v>
       </c>
       <c r="I62">
-        <f>$B$9*COS(2*E62-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>-3.3690773642174001</v>
       </c>
       <c r="J62">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>-3.1544397264088513</v>
       </c>
     </row>
@@ -11233,27 +11233,27 @@
         <v>5</v>
       </c>
       <c r="E63">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1.282282715750936</v>
       </c>
       <c r="F63" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>73.469387755102048</v>
       </c>
       <c r="G63">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H63">
-        <f>$B$9*COS(E63-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>-2.8022598781071619</v>
       </c>
       <c r="I63">
-        <f>$B$9*COS(2*E63-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>-2.0730326246000845</v>
       </c>
       <c r="J63">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>-2.161006788421532</v>
       </c>
     </row>
@@ -11262,27 +11262,27 @@
         <v>6</v>
       </c>
       <c r="E64">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1.5387392589011231</v>
       </c>
       <c r="F64" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>88.16326530612244</v>
       </c>
       <c r="G64">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H64">
-        <f>$B$9*COS(E64-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>-2.9215750935097029</v>
       </c>
       <c r="I64">
-        <f>$B$9*COS(2*E64-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>-0.24346683592671009</v>
       </c>
       <c r="J64">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>-0.45075621515069858</v>
       </c>
     </row>
@@ -11291,27 +11291,27 @@
         <v>7</v>
       </c>
       <c r="E65">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1.7951958020513104</v>
       </c>
       <c r="F65" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>102.85714285714286</v>
       </c>
       <c r="G65">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H65">
-        <f>$B$9*COS(E65-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>-2.8497892817622534</v>
       </c>
       <c r="I65">
-        <f>$B$9*COS(2*E65-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>1.6487582086467207</v>
       </c>
       <c r="J65">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1.5132546411701817</v>
       </c>
     </row>
@@ -11320,27 +11320,27 @@
         <v>8</v>
       </c>
       <c r="E66">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>2.0516523452014974</v>
       </c>
       <c r="F66" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>117.55102040816325</v>
       </c>
       <c r="G66">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H66">
-        <f>$B$9*COS(E66-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>-2.591597972474923</v>
       </c>
       <c r="I66">
-        <f>$B$9*COS(2*E66-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>3.1166545674684314</v>
       </c>
       <c r="J66">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>3.2393423092792228</v>
       </c>
     </row>
@@ -11349,27 +11349,27 @@
         <v>9</v>
       </c>
       <c r="E67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>2.3081088883516849</v>
       </c>
       <c r="F67" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>132.24489795918367</v>
       </c>
       <c r="G67">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H67">
-        <f>$B$9*COS(E67-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>-2.1638895299124603</v>
       </c>
       <c r="I67">
-        <f>$B$9*COS(2*E67-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>3.7824406292069535</v>
       </c>
       <c r="J67">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>4.332836813580208</v>
       </c>
     </row>
@@ -11378,27 +11378,27 @@
         <v>10</v>
       </c>
       <c r="E68">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>2.564565431501872</v>
       </c>
       <c r="F68" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>146.9387755102041</v>
       </c>
       <c r="G68">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H68">
-        <f>$B$9*COS(E68-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>-1.5946404804616034</v>
       </c>
       <c r="I68">
-        <f>$B$9*COS(2*E68-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>3.4747679674600875</v>
       </c>
       <c r="J68">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>4.5944132012841985</v>
       </c>
     </row>
@@ -11407,27 +11407,27 @@
         <v>11</v>
       </c>
       <c r="E69">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>2.8210219746520586</v>
       </c>
       <c r="F69" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>161.63265306122446</v>
       </c>
       <c r="G69">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H69">
-        <f>$B$9*COS(E69-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>-0.92108556037673894</v>
       </c>
       <c r="I69">
-        <f>$B$9*COS(2*E69-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>2.2728200158666239</v>
       </c>
       <c r="J69">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>4.0660201697755998</v>
       </c>
     </row>
@@ -11436,27 +11436,27 @@
         <v>12</v>
       </c>
       <c r="E70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>3.0774785178022461</v>
       </c>
       <c r="F70" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>176.32653061224488</v>
       </c>
       <c r="G70">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H70">
-        <f>$B$9*COS(E70-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>-0.18728218148208467</v>
       </c>
       <c r="I70">
-        <f>$B$9*COS(2*E70-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>0.48593321440112491</v>
       </c>
       <c r="J70">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>3.0129367472047548</v>
       </c>
     </row>
@@ -11465,27 +11465,27 @@
         <v>13</v>
       </c>
       <c r="E71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>3.3339350609524336</v>
       </c>
       <c r="F71" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>191.0204081632653</v>
       </c>
       <c r="G71">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H71">
-        <f>$B$9*COS(E71-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>0.55877137620401141</v>
       </c>
       <c r="I71">
-        <f>$B$9*COS(2*E71-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>-1.426014618541622</v>
       </c>
       <c r="J71">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1.8470424719481036</v>
       </c>
     </row>
@@ -11494,27 +11494,27 @@
         <v>14</v>
       </c>
       <c r="E72">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>3.5903916041026207</v>
       </c>
       <c r="F72" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>205.71428571428572</v>
       </c>
       <c r="G72">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H72">
-        <f>$B$9*COS(E72-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>1.268275545112862</v>
       </c>
       <c r="I72">
-        <f>$B$9*COS(2*E72-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>-2.9709596333785129</v>
       </c>
       <c r="J72">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1.0116016260200635</v>
       </c>
     </row>
@@ -11523,27 +11523,27 @@
         <v>15</v>
       </c>
       <c r="E73">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>3.8468481472528078</v>
       </c>
       <c r="F73" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>220.40816326530611</v>
       </c>
       <c r="G73">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H73">
-        <f>$B$9*COS(E73-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>1.894821463207381</v>
       </c>
       <c r="I73">
-        <f>$B$9*COS(2*E73-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>-3.7512907769749106</v>
       </c>
       <c r="J73">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>0.85781640051818497</v>
       </c>
     </row>
@@ -11552,27 +11552,27 @@
         <v>16</v>
       </c>
       <c r="E74">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>4.1033046904029948</v>
       </c>
       <c r="F74" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>235.10204081632651</v>
       </c>
       <c r="G74">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H74">
-        <f>$B$9*COS(E74-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>2.397426590360332</v>
       </c>
       <c r="I74">
-        <f>$B$9*COS(2*E74-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>-3.5661800037890905</v>
       </c>
       <c r="J74">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1.5455323008569555</v>
       </c>
     </row>
@@ -11581,27 +11581,27 @@
         <v>17</v>
       </c>
       <c r="E75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>4.3597612335531828</v>
       </c>
       <c r="F75" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>249.79591836734696</v>
       </c>
       <c r="G75">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H75">
-        <f>$B$9*COS(E75-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>2.7432153875300691</v>
       </c>
       <c r="I75">
-        <f>$B$9*COS(2*E75-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>-2.4632679021695938</v>
       </c>
       <c r="J75">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>2.9942331996461893</v>
       </c>
     </row>
@@ -11610,27 +11610,27 @@
         <v>18</v>
       </c>
       <c r="E76">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>4.6162177767033699</v>
       </c>
       <c r="F76" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>264.48979591836735</v>
       </c>
       <c r="G76">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H76">
-        <f>$B$9*COS(E76-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>2.9095697147745794</v>
       </c>
       <c r="I76">
-        <f>$B$9*COS(2*E76-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>-0.72640278906521305</v>
       </c>
       <c r="J76">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>4.8974526399950804</v>
       </c>
     </row>
@@ -11639,27 +11639,27 @@
         <v>19</v>
       </c>
       <c r="E77">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>4.872674319853556</v>
       </c>
       <c r="F77" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>279.18367346938771</v>
       </c>
       <c r="G77">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H77">
-        <f>$B$9*COS(E77-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>2.8856082899807012</v>
       </c>
       <c r="I77">
-        <f>$B$9*COS(2*E77-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>1.1974112284897527</v>
       </c>
       <c r="J77">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>6.7973052327561678</v>
       </c>
     </row>
@@ -11668,27 +11668,27 @@
         <v>20</v>
       </c>
       <c r="E78">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>5.129130863003744</v>
       </c>
       <c r="F78" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>293.87755102040819</v>
       </c>
       <c r="G78">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H78">
-        <f>$B$9*COS(E78-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>2.6728984365077597</v>
       </c>
       <c r="I78">
-        <f>$B$9*COS(2*E78-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>2.8130563888861988</v>
       </c>
       <c r="J78">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>8.2002405396796725</v>
       </c>
     </row>
@@ -11697,27 +11697,27 @@
         <v>21</v>
       </c>
       <c r="E79">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>5.3855874061539311</v>
       </c>
       <c r="F79" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>308.57142857142856</v>
       </c>
       <c r="G79">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H79">
-        <f>$B$9*COS(E79-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>2.2853535641373179</v>
       </c>
       <c r="I79">
-        <f>$B$9*COS(2*E79-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>3.7047260662909296</v>
       </c>
       <c r="J79">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>8.7043653447139615</v>
       </c>
     </row>
@@ -11726,27 +11726,27 @@
         <v>22</v>
       </c>
       <c r="E80">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>5.6420439493041172</v>
       </c>
       <c r="F80" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>323.26530612244892</v>
       </c>
       <c r="G80">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H80">
-        <f>$B$9*COS(E80-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>1.7483230891281722</v>
       </c>
       <c r="I80">
-        <f>$B$9*COS(2*E80-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>3.6429378415393132</v>
       </c>
       <c r="J80">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>8.1055466449532005</v>
       </c>
     </row>
@@ -11755,27 +11755,27 @@
         <v>23</v>
       </c>
       <c r="E81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>5.8985004924543052</v>
       </c>
       <c r="F81" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>337.9591836734694</v>
       </c>
       <c r="G81">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H81">
-        <f>$B$9*COS(E81-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>1.0969343219550949</v>
       </c>
       <c r="I81">
-        <f>$B$9*COS(2*E81-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>2.6435936922932508</v>
       </c>
       <c r="J81">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>6.4548137285340594</v>
       </c>
     </row>
@@ -11784,27 +11784,27 @@
         <v>24</v>
       </c>
       <c r="E82">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>6.1549570356044923</v>
       </c>
       <c r="F82" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>352.65306122448976</v>
       </c>
       <c r="G82">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="12"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H82">
-        <f>$B$9*COS(E82-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="13"/>
         <v>0.37379478030855762</v>
       </c>
       <c r="I82">
-        <f>$B$9*COS(2*E82-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="14"/>
         <v>0.96388741885613238</v>
       </c>
       <c r="J82">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>4.0519679134504045</v>
       </c>
     </row>
@@ -11856,15 +11856,15 @@
         <v>14.693877551020407</v>
       </c>
       <c r="G85">
-        <f>$B$9/$B$5</f>
+        <f t="shared" ref="G85:G108" si="18">$B$9/$B$5</f>
         <v>2.7142857142857144</v>
       </c>
       <c r="H85">
-        <f>$B$9*COS(E85-$B$10)/(1-$B$5)</f>
+        <f t="shared" ref="H85:H108" si="19">$B$9*COS(E85-$B$10)/(1-$B$5)</f>
         <v>-0.74145186065855972</v>
       </c>
       <c r="I85">
-        <f>$B$9*COS(2*E85-$B$11)/(4-$B$5)</f>
+        <f t="shared" ref="I85:I108" si="20">$B$9*COS(2*E85-$B$11)/(4-$B$5)</f>
         <v>-1.8647266976149641</v>
       </c>
       <c r="J85">
@@ -11883,27 +11883,27 @@
         <v>2</v>
       </c>
       <c r="E86">
-        <f t="shared" ref="E86:E108" si="12">D86*2*PI()/(24.5)</f>
+        <f t="shared" ref="E86:E108" si="21">D86*2*PI()/(24.5)</f>
         <v>0.51291308630037435</v>
       </c>
       <c r="F86" s="1">
-        <f t="shared" ref="F86:F108" si="13">E86*(180/PI())</f>
+        <f t="shared" ref="F86:F108" si="22">E86*(180/PI())</f>
         <v>29.387755102040813</v>
       </c>
       <c r="G86">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H86">
-        <f>$B$9*COS(E86-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>-1.4344051520115109</v>
       </c>
       <c r="I86">
-        <f>$B$9*COS(2*E86-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>-3.2495424994203157</v>
       </c>
       <c r="J86">
-        <f t="shared" ref="J86:J108" si="14">SUM(G86:I86)</f>
+        <f t="shared" ref="J86:J108" si="23">SUM(G86:I86)</f>
         <v>-1.9696619371461122</v>
       </c>
     </row>
@@ -11919,27 +11919,27 @@
         <v>3</v>
       </c>
       <c r="E87">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>0.76936962945056153</v>
       </c>
       <c r="F87" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>44.08163265306122</v>
       </c>
       <c r="G87">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H87">
-        <f>$B$9*COS(E87-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>-2.0335336094563448</v>
       </c>
       <c r="I87">
-        <f>$B$9*COS(2*E87-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>-3.7980476215626142</v>
       </c>
       <c r="J87">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>-3.1172955167332446</v>
       </c>
     </row>
@@ -11955,27 +11955,27 @@
         <v>4</v>
       </c>
       <c r="E88">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>1.0258261726007487</v>
       </c>
       <c r="F88" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>58.775510204081627</v>
       </c>
       <c r="G88">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H88">
-        <f>$B$9*COS(E88-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>-2.4996480764771656</v>
       </c>
       <c r="I88">
-        <f>$B$9*COS(2*E88-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>-3.3690773642174001</v>
       </c>
       <c r="J88">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>-3.1544397264088513</v>
       </c>
     </row>
@@ -11991,27 +11991,27 @@
         <v>5</v>
       </c>
       <c r="E89">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>1.282282715750936</v>
       </c>
       <c r="F89" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>73.469387755102048</v>
       </c>
       <c r="G89">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H89">
-        <f>$B$9*COS(E89-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>-2.8022598781071619</v>
       </c>
       <c r="I89">
-        <f>$B$9*COS(2*E89-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>-2.0730326246000845</v>
       </c>
       <c r="J89">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>-2.161006788421532</v>
       </c>
     </row>
@@ -12020,27 +12020,27 @@
         <v>6</v>
       </c>
       <c r="E90">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>1.5387392589011231</v>
       </c>
       <c r="F90" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>88.16326530612244</v>
       </c>
       <c r="G90">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H90">
-        <f>$B$9*COS(E90-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>-2.9215750935097029</v>
       </c>
       <c r="I90">
-        <f>$B$9*COS(2*E90-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>-0.24346683592671009</v>
       </c>
       <c r="J90">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>-0.45075621515069858</v>
       </c>
     </row>
@@ -12049,27 +12049,27 @@
         <v>7</v>
       </c>
       <c r="E91">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>1.7951958020513104</v>
       </c>
       <c r="F91" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>102.85714285714286</v>
       </c>
       <c r="G91">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H91">
-        <f>$B$9*COS(E91-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>-2.8497892817622534</v>
       </c>
       <c r="I91">
-        <f>$B$9*COS(2*E91-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>1.6487582086467207</v>
       </c>
       <c r="J91">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>1.5132546411701817</v>
       </c>
     </row>
@@ -12078,27 +12078,27 @@
         <v>8</v>
       </c>
       <c r="E92">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>2.0516523452014974</v>
       </c>
       <c r="F92" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>117.55102040816325</v>
       </c>
       <c r="G92">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H92">
-        <f>$B$9*COS(E92-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>-2.591597972474923</v>
       </c>
       <c r="I92">
-        <f>$B$9*COS(2*E92-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>3.1166545674684314</v>
       </c>
       <c r="J92">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>3.2393423092792228</v>
       </c>
     </row>
@@ -12107,27 +12107,27 @@
         <v>9</v>
       </c>
       <c r="E93">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>2.3081088883516849</v>
       </c>
       <c r="F93" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>132.24489795918367</v>
       </c>
       <c r="G93">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H93">
-        <f>$B$9*COS(E93-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>-2.1638895299124603</v>
       </c>
       <c r="I93">
-        <f>$B$9*COS(2*E93-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>3.7824406292069535</v>
       </c>
       <c r="J93">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>4.332836813580208</v>
       </c>
     </row>
@@ -12136,27 +12136,27 @@
         <v>10</v>
       </c>
       <c r="E94">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>2.564565431501872</v>
       </c>
       <c r="F94" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>146.9387755102041</v>
       </c>
       <c r="G94">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H94">
-        <f>$B$9*COS(E94-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>-1.5946404804616034</v>
       </c>
       <c r="I94">
-        <f>$B$9*COS(2*E94-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>3.4747679674600875</v>
       </c>
       <c r="J94">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>4.5944132012841985</v>
       </c>
     </row>
@@ -12165,27 +12165,27 @@
         <v>11</v>
       </c>
       <c r="E95">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>2.8210219746520586</v>
       </c>
       <c r="F95" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>161.63265306122446</v>
       </c>
       <c r="G95">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H95">
-        <f>$B$9*COS(E95-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>-0.92108556037673894</v>
       </c>
       <c r="I95">
-        <f>$B$9*COS(2*E95-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>2.2728200158666239</v>
       </c>
       <c r="J95">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>4.0660201697755998</v>
       </c>
     </row>
@@ -12194,27 +12194,27 @@
         <v>12</v>
       </c>
       <c r="E96">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>3.0774785178022461</v>
       </c>
       <c r="F96" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>176.32653061224488</v>
       </c>
       <c r="G96">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H96">
-        <f>$B$9*COS(E96-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>-0.18728218148208467</v>
       </c>
       <c r="I96">
-        <f>$B$9*COS(2*E96-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>0.48593321440112491</v>
       </c>
       <c r="J96">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>3.0129367472047548</v>
       </c>
     </row>
@@ -12223,27 +12223,27 @@
         <v>13</v>
       </c>
       <c r="E97">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>3.3339350609524336</v>
       </c>
       <c r="F97" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>191.0204081632653</v>
       </c>
       <c r="G97">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H97">
-        <f>$B$9*COS(E97-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>0.55877137620401141</v>
       </c>
       <c r="I97">
-        <f>$B$9*COS(2*E97-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>-1.426014618541622</v>
       </c>
       <c r="J97">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>1.8470424719481036</v>
       </c>
     </row>
@@ -12252,27 +12252,27 @@
         <v>14</v>
       </c>
       <c r="E98">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>3.5903916041026207</v>
       </c>
       <c r="F98" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>205.71428571428572</v>
       </c>
       <c r="G98">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H98">
-        <f>$B$9*COS(E98-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>1.268275545112862</v>
       </c>
       <c r="I98">
-        <f>$B$9*COS(2*E98-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>-2.9709596333785129</v>
       </c>
       <c r="J98">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>1.0116016260200635</v>
       </c>
     </row>
@@ -12281,27 +12281,27 @@
         <v>15</v>
       </c>
       <c r="E99">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>3.8468481472528078</v>
       </c>
       <c r="F99" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>220.40816326530611</v>
       </c>
       <c r="G99">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H99">
-        <f>$B$9*COS(E99-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>1.894821463207381</v>
       </c>
       <c r="I99">
-        <f>$B$9*COS(2*E99-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>-3.7512907769749106</v>
       </c>
       <c r="J99">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>0.85781640051818497</v>
       </c>
     </row>
@@ -12310,27 +12310,27 @@
         <v>16</v>
       </c>
       <c r="E100">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>4.1033046904029948</v>
       </c>
       <c r="F100" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>235.10204081632651</v>
       </c>
       <c r="G100">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H100">
-        <f>$B$9*COS(E100-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>2.397426590360332</v>
       </c>
       <c r="I100">
-        <f>$B$9*COS(2*E100-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>-3.5661800037890905</v>
       </c>
       <c r="J100">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>1.5455323008569555</v>
       </c>
     </row>
@@ -12339,27 +12339,27 @@
         <v>17</v>
       </c>
       <c r="E101">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>4.3597612335531828</v>
       </c>
       <c r="F101" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>249.79591836734696</v>
       </c>
       <c r="G101">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H101">
-        <f>$B$9*COS(E101-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>2.7432153875300691</v>
       </c>
       <c r="I101">
-        <f>$B$9*COS(2*E101-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>-2.4632679021695938</v>
       </c>
       <c r="J101">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>2.9942331996461893</v>
       </c>
     </row>
@@ -12368,27 +12368,27 @@
         <v>18</v>
       </c>
       <c r="E102">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>4.6162177767033699</v>
       </c>
       <c r="F102" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>264.48979591836735</v>
       </c>
       <c r="G102">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H102">
-        <f>$B$9*COS(E102-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>2.9095697147745794</v>
       </c>
       <c r="I102">
-        <f>$B$9*COS(2*E102-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>-0.72640278906521305</v>
       </c>
       <c r="J102">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>4.8974526399950804</v>
       </c>
     </row>
@@ -12397,27 +12397,27 @@
         <v>19</v>
       </c>
       <c r="E103">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>4.872674319853556</v>
       </c>
       <c r="F103" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>279.18367346938771</v>
       </c>
       <c r="G103">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H103">
-        <f>$B$9*COS(E103-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>2.8856082899807012</v>
       </c>
       <c r="I103">
-        <f>$B$9*COS(2*E103-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>1.1974112284897527</v>
       </c>
       <c r="J103">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>6.7973052327561678</v>
       </c>
     </row>
@@ -12426,27 +12426,27 @@
         <v>20</v>
       </c>
       <c r="E104">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>5.129130863003744</v>
       </c>
       <c r="F104" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>293.87755102040819</v>
       </c>
       <c r="G104">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H104">
-        <f>$B$9*COS(E104-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>2.6728984365077597</v>
       </c>
       <c r="I104">
-        <f>$B$9*COS(2*E104-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>2.8130563888861988</v>
       </c>
       <c r="J104">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>8.2002405396796725</v>
       </c>
     </row>
@@ -12455,27 +12455,27 @@
         <v>21</v>
       </c>
       <c r="E105">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>5.3855874061539311</v>
       </c>
       <c r="F105" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>308.57142857142856</v>
       </c>
       <c r="G105">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H105">
-        <f>$B$9*COS(E105-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>2.2853535641373179</v>
       </c>
       <c r="I105">
-        <f>$B$9*COS(2*E105-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>3.7047260662909296</v>
       </c>
       <c r="J105">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>8.7043653447139615</v>
       </c>
     </row>
@@ -12484,27 +12484,27 @@
         <v>22</v>
       </c>
       <c r="E106">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>5.6420439493041172</v>
       </c>
       <c r="F106" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>323.26530612244892</v>
       </c>
       <c r="G106">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H106">
-        <f>$B$9*COS(E106-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>1.7483230891281722</v>
       </c>
       <c r="I106">
-        <f>$B$9*COS(2*E106-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>3.6429378415393132</v>
       </c>
       <c r="J106">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>8.1055466449532005</v>
       </c>
     </row>
@@ -12513,27 +12513,27 @@
         <v>23</v>
       </c>
       <c r="E107">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>5.8985004924543052</v>
       </c>
       <c r="F107" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>337.9591836734694</v>
       </c>
       <c r="G107">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H107">
-        <f>$B$9*COS(E107-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>1.0969343219550949</v>
       </c>
       <c r="I107">
-        <f>$B$9*COS(2*E107-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>2.6435936922932508</v>
       </c>
       <c r="J107">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>6.4548137285340594</v>
       </c>
     </row>
@@ -12542,27 +12542,27 @@
         <v>24</v>
       </c>
       <c r="E108">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>6.1549570356044923</v>
       </c>
       <c r="F108" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>352.65306122448976</v>
       </c>
       <c r="G108">
-        <f>$B$9/$B$5</f>
+        <f t="shared" si="18"/>
         <v>2.7142857142857144</v>
       </c>
       <c r="H108">
-        <f>$B$9*COS(E108-$B$10)/(1-$B$5)</f>
+        <f t="shared" si="19"/>
         <v>0.37379478030855762</v>
       </c>
       <c r="I108">
-        <f>$B$9*COS(2*E108-$B$11)/(4-$B$5)</f>
+        <f t="shared" si="20"/>
         <v>0.96388741885613238</v>
       </c>
       <c r="J108">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>4.0519679134504045</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working on COD fits
</commit_message>
<xml_diff>
--- a/ToyQuadScan.xlsx
+++ b/ToyQuadScan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelgrant/Documents/gm2/EDM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AA715C-8302-FF46-9E3F-1AE3800A1721}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6AFB89C-05B2-E346-B90F-9B48B986A9E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{1274A7F7-32CE-AC49-AA55-A5E18D405CEC}"/>
   </bookViews>
@@ -8979,7 +8979,7 @@
   <dimension ref="B1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="B1:K14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>